<commit_message>
fix typo in dataset
</commit_message>
<xml_diff>
--- a/ImportDB/Utown Food Menu Dataset.xlsx
+++ b/ImportDB/Utown Food Menu Dataset.xlsx
@@ -1187,7 +1187,7 @@
     <t>Bandung</t>
   </si>
   <si>
-    <t>gs://orbitaroundfood.appspot.com/bandung.jpeg</t>
+    <t>gs://orbitaroundfood.appspot.com/bandung.jpg</t>
   </si>
   <si>
     <t>Fresh Soya Bean</t>
@@ -14949,7 +14949,7 @@
       <c r="C358" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="D358" s="5" t="s">
+      <c r="D358" s="8" t="s">
         <v>391</v>
       </c>
       <c r="E358" s="5" t="s">

</xml_diff>